<commit_message>
Added remaining tables and started working on them
</commit_message>
<xml_diff>
--- a/SQL Collection/DataBaseRecords.xlsx
+++ b/SQL Collection/DataBaseRecords.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lijani\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lijani\Documents\GitHub\PremierService-Solutions-FrontEnd\SQL Collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0CC27D-2165-47A3-9AB9-B719B61BE770}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A285BF-2F07-430E-AF45-1401AB0A07C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="832" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Address" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,19 @@
     <sheet name="ServiceRequest" sheetId="10" r:id="rId9"/>
     <sheet name="Job" sheetId="11" r:id="rId10"/>
     <sheet name="Contract" sheetId="27" r:id="rId11"/>
+    <sheet name="ContractState" sheetId="38" r:id="rId12"/>
+    <sheet name="ClientContractLink" sheetId="29" r:id="rId13"/>
+    <sheet name="ClientBusinessEmployee" sheetId="28" r:id="rId14"/>
+    <sheet name="JobEmployeeLink" sheetId="30" r:id="rId15"/>
+    <sheet name="ServiceContractLink" sheetId="31" r:id="rId16"/>
+    <sheet name="ServiceContractStateLink" sheetId="32" r:id="rId17"/>
+    <sheet name="ServicePackageLink" sheetId="33" r:id="rId18"/>
+    <sheet name="ServicePackageStateLink" sheetId="34" r:id="rId19"/>
+    <sheet name="ServiceRequestJobLink" sheetId="35" r:id="rId20"/>
+    <sheet name="ServiceRequestSpecialisationLin" sheetId="36" r:id="rId21"/>
+    <sheet name="SpecialisationEmployeeLink" sheetId="37" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -67,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="610">
   <si>
     <t>streetName</t>
   </si>
@@ -1462,6 +1472,441 @@
   </si>
   <si>
     <t>20</t>
+  </si>
+  <si>
+    <t>2004/05/25</t>
+  </si>
+  <si>
+    <t>2005/05/25</t>
+  </si>
+  <si>
+    <t>2008/10/20</t>
+  </si>
+  <si>
+    <t>2010/10/20</t>
+  </si>
+  <si>
+    <t>2015/01/01</t>
+  </si>
+  <si>
+    <t>2015/12/31</t>
+  </si>
+  <si>
+    <t>2016/01/01</t>
+  </si>
+  <si>
+    <t>2018/12/31</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2017/05/01</t>
+  </si>
+  <si>
+    <t>2020/10/01</t>
+  </si>
+  <si>
+    <t>Building Maintenance</t>
+  </si>
+  <si>
+    <t>Garden Maintenance</t>
+  </si>
+  <si>
+    <t>General Equipment Maintenance</t>
+  </si>
+  <si>
+    <t>Office Equipment Maintenance</t>
+  </si>
+  <si>
+    <t>Communication Equipment Maintenance</t>
+  </si>
+  <si>
+    <t>2019/01/01</t>
+  </si>
+  <si>
+    <t>2020/05/31</t>
+  </si>
+  <si>
+    <t>2021/05/31</t>
+  </si>
+  <si>
+    <t>Property Maintenace</t>
+  </si>
+  <si>
+    <t>2020/06/01</t>
+  </si>
+  <si>
+    <t>2022/06/01</t>
+  </si>
+  <si>
+    <t>2020/01/01</t>
+  </si>
+  <si>
+    <t>2022/12/31</t>
+  </si>
+  <si>
+    <t>Wireless Connectivity Maintenance</t>
+  </si>
+  <si>
+    <t>2021/04/20</t>
+  </si>
+  <si>
+    <t>2023/04/20</t>
+  </si>
+  <si>
+    <t>2021/05/01</t>
+  </si>
+  <si>
+    <t>2021/05/19</t>
+  </si>
+  <si>
+    <t>Bathroom Repairs</t>
+  </si>
+  <si>
+    <t>Routine Maintenance</t>
+  </si>
+  <si>
+    <t>2022/01/01</t>
+  </si>
+  <si>
+    <t>2021/02/01</t>
+  </si>
+  <si>
+    <t>businessID</t>
+  </si>
+  <si>
+    <t>contractID</t>
+  </si>
+  <si>
+    <t>clientIndividualID</t>
+  </si>
+  <si>
+    <t>clientBusinessID</t>
+  </si>
+  <si>
+    <t>jobID</t>
+  </si>
+  <si>
+    <t>servicePackageID</t>
+  </si>
+  <si>
+    <t>serviceID</t>
+  </si>
+  <si>
+    <t>serviceRequestID</t>
+  </si>
+  <si>
+    <t>specialisationRequiredID</t>
+  </si>
+  <si>
+    <t>specialisationID</t>
+  </si>
+  <si>
+    <t>Liam</t>
+  </si>
+  <si>
+    <t>Stevens</t>
+  </si>
+  <si>
+    <t>0870120506</t>
+  </si>
+  <si>
+    <t>stevens.liam@gmail.com</t>
+  </si>
+  <si>
+    <t>9010100056023</t>
+  </si>
+  <si>
+    <t>1990/10/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicole </t>
+  </si>
+  <si>
+    <t>Horwood</t>
+  </si>
+  <si>
+    <t>0761154212</t>
+  </si>
+  <si>
+    <t>horwood@hotmail.com</t>
+  </si>
+  <si>
+    <t>8912120023086</t>
+  </si>
+  <si>
+    <t>1989/12/12</t>
+  </si>
+  <si>
+    <t>Nicholas</t>
+  </si>
+  <si>
+    <t>0764451233</t>
+  </si>
+  <si>
+    <t>horwood1@hotmail.com</t>
+  </si>
+  <si>
+    <t>8704040056088</t>
+  </si>
+  <si>
+    <t>1987/04/04</t>
+  </si>
+  <si>
+    <t>oldContractID</t>
+  </si>
+  <si>
+    <t>2005/01/25</t>
+  </si>
+  <si>
+    <t>2005/05/20</t>
+  </si>
+  <si>
+    <t>45000</t>
+  </si>
+  <si>
+    <t>2009/10/20</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>40000</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>16000</t>
+  </si>
+  <si>
+    <t>14000</t>
+  </si>
+  <si>
+    <t>15800</t>
+  </si>
+  <si>
+    <t>2021/10/31</t>
+  </si>
+  <si>
+    <t>2019/10/01</t>
+  </si>
+  <si>
+    <t>17000</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>2021/05/28</t>
+  </si>
+  <si>
+    <t>2020/10/31</t>
+  </si>
+  <si>
+    <t>GOL4</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>8000</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>2022/01/31</t>
+  </si>
+  <si>
+    <t>14500</t>
+  </si>
+  <si>
+    <t>18000</t>
+  </si>
+  <si>
+    <t>13000</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t>Telemarketing</t>
+  </si>
+  <si>
+    <t>0457894562</t>
+  </si>
+  <si>
+    <t>samsam@gmail.com</t>
+  </si>
+  <si>
+    <t>Juniper</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>0784561111</t>
+  </si>
+  <si>
+    <t>junefri@gmail.com</t>
+  </si>
+  <si>
+    <t>Greg</t>
+  </si>
+  <si>
+    <t>Hall</t>
+  </si>
+  <si>
+    <t>Garden Manager</t>
+  </si>
+  <si>
+    <t>0752369874</t>
+  </si>
+  <si>
+    <t>hallman@hotmail.com</t>
+  </si>
+  <si>
+    <t>Hayley</t>
+  </si>
+  <si>
+    <t>Shae</t>
+  </si>
+  <si>
+    <t>Plumber</t>
+  </si>
+  <si>
+    <t>0784568899</t>
+  </si>
+  <si>
+    <t>shae.hayley@gmail.com</t>
+  </si>
+  <si>
+    <t>Miena</t>
+  </si>
+  <si>
+    <t>van der Vyver</t>
+  </si>
+  <si>
+    <t>0568974555</t>
+  </si>
+  <si>
+    <t>vdv.miena@vodamail.com</t>
+  </si>
+  <si>
+    <t>Amanda</t>
+  </si>
+  <si>
+    <t>Finances</t>
+  </si>
+  <si>
+    <t>0824569874</t>
+  </si>
+  <si>
+    <t>amanda@industries.co.za</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Bush</t>
+  </si>
+  <si>
+    <t>Cleaning Manager</t>
+  </si>
+  <si>
+    <t>0786541200</t>
+  </si>
+  <si>
+    <t>bushman@gmail.com</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Morrison</t>
+  </si>
+  <si>
+    <t>0825994455</t>
+  </si>
+  <si>
+    <t>olivia@hotmail.com</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>0687458985</t>
+  </si>
+  <si>
+    <t>paulhougton@gmail.com</t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t>0865641233</t>
+  </si>
+  <si>
+    <t>venter.michelle@gmail.com</t>
+  </si>
+  <si>
+    <t>Bernadette</t>
+  </si>
+  <si>
+    <t>Trello</t>
+  </si>
+  <si>
+    <t>Site Manager</t>
+  </si>
+  <si>
+    <t>0456987777</t>
+  </si>
+  <si>
+    <t>bernie.trello@gmail.com</t>
+  </si>
+  <si>
+    <t>Junanda</t>
+  </si>
+  <si>
+    <t>Bojangle</t>
+  </si>
+  <si>
+    <t>0754123384</t>
+  </si>
+  <si>
+    <t>bojangles@gmail.com</t>
+  </si>
+  <si>
+    <t>Ashley</t>
+  </si>
+  <si>
+    <t>Jillian</t>
+  </si>
+  <si>
+    <t>0785641255</t>
+  </si>
+  <si>
+    <t>jill.ash@gmail.com</t>
+  </si>
+  <si>
+    <t>Carey</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>0764451115</t>
+  </si>
+  <si>
+    <t>kingcar@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1811,7 +2256,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2123,8 +2568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213B5DE8-4E16-41E8-BDD7-94A9F8EA519D}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2335,8 +2780,8 @@
       <c r="E10" s="2">
         <v>6</v>
       </c>
-      <c r="F10" s="2">
-        <v>5</v>
+      <c r="F10" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2355,8 +2800,8 @@
       <c r="E11" s="2">
         <v>8</v>
       </c>
-      <c r="F11" s="2">
-        <v>6</v>
+      <c r="F11" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2395,8 +2840,8 @@
       <c r="E13" s="2">
         <v>9</v>
       </c>
-      <c r="F13" s="2">
-        <v>5</v>
+      <c r="F13" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2595,8 +3040,8 @@
       <c r="E23" s="2">
         <v>12</v>
       </c>
-      <c r="F23" s="2">
-        <v>6</v>
+      <c r="F23" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2635,8 +3080,8 @@
       <c r="E25" s="2">
         <v>11</v>
       </c>
-      <c r="F25" s="2">
-        <v>4</v>
+      <c r="F25" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2655,8 +3100,8 @@
       <c r="E26" s="2">
         <v>7</v>
       </c>
-      <c r="F26" s="2">
-        <v>5</v>
+      <c r="F26" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2729,8 +3174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A729D5E5-EBA3-4AD4-89B3-6D680D0AD05C}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2738,7 +3183,7 @@
     <col min="1" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
     <col min="4" max="5" width="27.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2762,124 +3207,246 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -2992,6 +3559,1846 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB588B5-A09D-41B5-A4E7-FD14543CAC90}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="G14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="G17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="G18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="G19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="G20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="G21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="G22">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033902A5-014A-4552-A1FB-B251320F8B86}">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87AD4437-4633-4DCE-98BC-91A091D5F0E2}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>609</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{5A9AE0AA-1E55-4AAC-BE90-9F96E72B949C}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{64E0B0B3-2BFC-49E8-B86F-CCC9FBBE7B0A}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{B2F72C7D-2320-4897-AA99-19FC99B680FB}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{2F2CC61C-5EE5-4F2C-9761-5D56109870E8}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{37A9B7FB-EEA6-49D9-A74F-8DCE710D97D2}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{D67777CD-AF48-4DA3-BE77-D2B082280422}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{CF50BE1A-CB85-4806-889C-908A6DF3C033}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{A2F7E3DE-C308-4874-B05B-D65346EE31DD}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{C8E9B577-CD89-4E7D-8EED-1940202C2AF4}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{EB5B5328-F817-41B1-B456-48FECAC2F08C}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{E10CCC6D-E798-487A-94BB-EF96F3E4A6CB}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{61C679BE-55F0-4070-B129-9A358EC61BA4}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{37B32ED7-961B-45F2-9FCD-C171B206F6A4}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{ECB03443-B4EA-48EB-BAED-74A53C235AE8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8B04A5-8130-4B55-B0CE-739B0F513F4F}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54DDE06A-2485-41CD-A4A8-C5870EE7DB1B}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49883B9-D961-4522-BC6F-FD0430E0BD73}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888CC129-151D-49F2-9EB6-6322C996EB93}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E74FC7F-785F-42AF-A035-14EA8387704C}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3003,15 +5410,15 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
@@ -3136,115 +5543,115 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>134</v>
+        <v>113</v>
+      </c>
+      <c r="C5" s="2">
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
+        <v>339</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2">
-        <v>5</v>
+      <c r="A6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>144</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>27</v>
+        <v>341</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="2">
-        <v>6</v>
+      <c r="A7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>115</v>
+        <v>158</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I7" t="s">
+        <v>147</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="2">
-        <v>10</v>
+      <c r="A8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>164</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1</v>
+        <v>343</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>27</v>
@@ -3252,83 +5659,83 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>147</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>158</v>
+        <v>190</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>159</v>
+        <v>191</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>160</v>
+        <v>192</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>147</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>161</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>147</v>
@@ -3339,25 +5746,25 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>167</v>
+        <v>508</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>168</v>
+        <v>509</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>170</v>
+        <v>461</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>171</v>
+        <v>510</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>172</v>
+        <v>511</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>173</v>
+        <v>512</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>344</v>
+        <v>513</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>147</v>
@@ -3368,25 +5775,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>174</v>
+        <v>514</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>175</v>
+        <v>515</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>189</v>
+        <v>259</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>190</v>
+        <v>516</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>191</v>
+        <v>517</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>192</v>
+        <v>518</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>345</v>
+        <v>519</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>147</v>
@@ -3397,65 +5804,119 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>520</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>193</v>
+        <v>515</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>194</v>
+        <v>259</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>195</v>
+        <v>521</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>196</v>
+        <v>522</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>197</v>
+        <v>523</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>346</v>
+        <v>524</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="A17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="2">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -3463,17 +5924,449 @@
     <hyperlink ref="E2" r:id="rId1" xr:uid="{823BB252-E784-4809-9491-8163236AC9CE}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{91822FBF-8BBC-46E8-AD23-268479C18DF2}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{31AD3656-8BD8-4E53-93F3-4E6D9B0F3726}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{9C713FE9-3584-44D3-A948-B3D59640D65B}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{17631E80-A551-4CF4-B424-0AE6775C57A1}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{69B30157-E0C9-4862-AB13-30420E3A6EE1}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{2BFCB5C5-8FD0-454F-B6F2-586404801100}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{5A160CA0-6E5B-4C54-BD33-C27437F93ED2}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{40A56487-E364-4986-BDC4-27654463D6B9}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{748C7818-FA16-4F0A-8267-8A53AF2EC6CA}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{D0DFE2B2-B677-4761-B70B-53A26BC92367}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{70559EC6-B895-40D6-8E5B-175C04F90B5C}"/>
-    <hyperlink ref="E14" r:id="rId13" xr:uid="{73625884-7EB2-4B83-911E-CD60E57C5232}"/>
+    <hyperlink ref="E15" r:id="rId4" xr:uid="{9C713FE9-3584-44D3-A948-B3D59640D65B}"/>
+    <hyperlink ref="E16" r:id="rId5" xr:uid="{17631E80-A551-4CF4-B424-0AE6775C57A1}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{69B30157-E0C9-4862-AB13-30420E3A6EE1}"/>
+    <hyperlink ref="E17" r:id="rId7" xr:uid="{2BFCB5C5-8FD0-454F-B6F2-586404801100}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{5A160CA0-6E5B-4C54-BD33-C27437F93ED2}"/>
+    <hyperlink ref="E7" r:id="rId9" xr:uid="{40A56487-E364-4986-BDC4-27654463D6B9}"/>
+    <hyperlink ref="E8" r:id="rId10" xr:uid="{748C7818-FA16-4F0A-8267-8A53AF2EC6CA}"/>
+    <hyperlink ref="E9" r:id="rId11" xr:uid="{D0DFE2B2-B677-4761-B70B-53A26BC92367}"/>
+    <hyperlink ref="E10" r:id="rId12" xr:uid="{70559EC6-B895-40D6-8E5B-175C04F90B5C}"/>
+    <hyperlink ref="E11" r:id="rId13" xr:uid="{73625884-7EB2-4B83-911E-CD60E57C5232}"/>
+    <hyperlink ref="E12" r:id="rId14" xr:uid="{9F8DF21B-BED4-40FA-9AF7-32C7CF371229}"/>
+    <hyperlink ref="E13" r:id="rId15" xr:uid="{F9254FBC-69CC-49FA-B12E-9E4ED518C405}"/>
+    <hyperlink ref="E14" r:id="rId16" xr:uid="{CA37763E-C5EE-4011-9FDE-908238603EBC}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB8D7C6-0240-4ECE-BE64-2CC85BE3FEFC}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC62D1D-0EA8-4378-9170-EAD7A092500C}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A2597C-F110-4421-AB34-615295043718}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>